<commit_message>
add DuoPods / Yarbrough08 / start work on RealFuels
</commit_message>
<xml_diff>
--- a/docs/ResourceMassPerEC.xlsx
+++ b/docs/ResourceMassPerEC.xlsx
@@ -29,7 +29,7 @@
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="B27" authorId="0" shapeId="0">
+    <comment ref="B30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C27" authorId="0" shapeId="0">
+    <comment ref="C30" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="58">
   <si>
     <t>FD = 1 / (F1c+F2c+f3c)</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>battery</t>
+  </si>
+  <si>
+    <t>US</t>
   </si>
 </sst>
 </file>
@@ -527,13 +530,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>88</xdr:row>
+      <xdr:row>91</xdr:row>
       <xdr:rowOff>152399</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>122</xdr:row>
+      <xdr:row>125</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -4082,10 +4085,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X86"/>
+  <dimension ref="A1:X89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" workbookViewId="0">
-      <selection activeCell="E69" sqref="E69:E74"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4949,429 +4952,504 @@
       <c r="W24" s="3"/>
       <c r="X24" s="12"/>
     </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="B25" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6">
+        <v>6</v>
+      </c>
+      <c r="E25" s="5">
+        <f>SUM(E26:E27)</f>
+        <v>3.7499999999999999E-3</v>
+      </c>
+      <c r="F25" s="5">
+        <f>D25/E25</f>
+        <v>1600</v>
+      </c>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="6"/>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+      <c r="X25" s="6"/>
+    </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="6"/>
+      <c r="D26" s="1">
+        <f>E26/E25</f>
+        <v>0.45</v>
+      </c>
+      <c r="E26" s="6">
+        <f>G26/D25</f>
+        <v>1.6875E-3</v>
+      </c>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6">
+        <v>1.0125E-2</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+      <c r="U26" s="6"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
+      <c r="X26" s="6"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="6"/>
+      <c r="D27" s="1">
+        <f>E27/E25</f>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="E27" s="6">
+        <f>G27/D25</f>
+        <v>2.0625000000000001E-3</v>
+      </c>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6">
+        <v>1.2375000000000001E-2</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+      <c r="U27" s="6"/>
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="6"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="32">
+      <c r="B30" s="32">
         <v>1</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C30" s="5">
         <v>1.5</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G30" s="1">
         <v>0.33364751877527898</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A28" s="9"/>
-      <c r="B28" s="6" t="s">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="1">
-        <f>C27/D8</f>
+      <c r="C31" s="6"/>
+      <c r="D31" s="1">
+        <f>C30/D8</f>
         <v>1.5</v>
       </c>
-      <c r="E28" s="1">
-        <f>E9*D28*B$27</f>
+      <c r="E31" s="1">
+        <f>E9*D31*B$30</f>
         <v>1.6874999999999998E-3</v>
-      </c>
-    </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
-      <c r="B29" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="1">
-        <f>C27/D9</f>
-        <v>3.3333333333333335</v>
-      </c>
-      <c r="E29" s="1">
-        <f>E10*D29*B$27</f>
-        <v>4.5833333333333342E-3</v>
-      </c>
-      <c r="G29" s="1">
-        <v>0.17061520846463141</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A30" s="11"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="I30" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B31" s="32">
-        <v>1</v>
-      </c>
-      <c r="C31" s="5">
-        <f>$C$27</f>
-        <v>1.5</v>
-      </c>
-      <c r="D31" s="1">
-        <f>C31/D12</f>
-        <v>1.5</v>
-      </c>
-      <c r="E31" s="1">
-        <f>E12*D31*B$31</f>
-        <v>1.5E-3</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="B32" s="6" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
       <c r="C32" s="6"/>
-      <c r="G32" s="17">
+      <c r="D32" s="1">
+        <f>C30/D9</f>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="E32" s="1">
+        <f>E10*D32*B$30</f>
+        <v>4.5833333333333342E-3</v>
+      </c>
+      <c r="G32" s="1">
         <v>0.17061520846463141</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="11"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
-      <c r="G33" s="17">
-        <v>8.5849656749061198E-2</v>
+      <c r="I33" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>11</v>
+      <c r="A34" s="4" t="s">
+        <v>13</v>
       </c>
       <c r="B34" s="32">
         <v>1</v>
       </c>
       <c r="C34" s="5">
-        <f>$C$27</f>
+        <f>$C$30</f>
         <v>1.5</v>
       </c>
-      <c r="G34" s="17">
+      <c r="D34" s="1">
+        <f>C34/D12</f>
+        <v>1.5</v>
+      </c>
+      <c r="E34" s="1">
+        <f>E12*D34*B$34</f>
+        <v>1.5E-3</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
+      <c r="B35" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C35" s="6"/>
+      <c r="G35" s="17">
+        <v>0.17061520846463141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="G36" s="17">
+        <v>8.5849656749061198E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B37" s="32">
+        <v>1</v>
+      </c>
+      <c r="C37" s="5">
+        <f>$C$30</f>
+        <v>1.5</v>
+      </c>
+      <c r="G37" s="17">
         <v>1.3801405443121E-4</v>
       </c>
-      <c r="J34" s="22" t="s">
+      <c r="J37" s="22" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B35" s="6" t="s">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B38" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="1">
-        <f>C34/D15</f>
+      <c r="C38" s="6"/>
+      <c r="D38" s="1">
+        <f>C37/D15</f>
         <v>1.5</v>
       </c>
-      <c r="E35" s="1">
-        <f>E16*D35*B$34</f>
+      <c r="E38" s="1">
+        <f>E16*D38*B$37</f>
         <v>0.31279454885182406</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="9"/>
-      <c r="B36" s="6" t="s">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
+      <c r="B39" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C36" s="6"/>
-      <c r="D36" s="1">
-        <f>C34/D16</f>
+      <c r="C39" s="6"/>
+      <c r="D39" s="1">
+        <f>C37/D16</f>
         <v>2.2547655703289005</v>
       </c>
-      <c r="E36" s="1">
-        <f>E17*D36*B$34</f>
+      <c r="E39" s="1">
+        <f>E17*D39*B$37</f>
         <v>0.23658659476507876</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="9"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="6"/>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="9"/>
-      <c r="B38" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="D38" s="1">
-        <f>C34/D15</f>
-        <v>1.5</v>
-      </c>
-      <c r="E38" s="33">
-        <f>E19*D38*B$34</f>
-        <v>2.5302576645721783E-4</v>
-      </c>
-      <c r="G38" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="H38" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="I38" s="1">
-        <v>0.33364751877527898</v>
-      </c>
-      <c r="J38" s="1">
-        <f>I38/G38</f>
-        <v>0.20852969923454936</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="11"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="3"/>
-      <c r="H39" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="I39" s="1">
-        <v>0.167883773198164</v>
-      </c>
-      <c r="J39" s="1">
-        <f>I39/G38</f>
-        <v>0.10492735824885249</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>49</v>
-      </c>
-    </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B40" s="32">
-        <v>1</v>
-      </c>
-      <c r="C40" s="5">
-        <f>$C$27</f>
-        <v>1.5</v>
-      </c>
-      <c r="H40" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="I40" s="1">
-        <v>2.69894150887699E-4</v>
-      </c>
-      <c r="J40" s="1">
-        <f>I40/G38</f>
-        <v>1.6868384430481187E-4</v>
-      </c>
+      <c r="A40" s="9"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="9"/>
       <c r="B41" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" s="1">
+        <f>C37/D15</f>
+        <v>1.5</v>
+      </c>
+      <c r="E41" s="33">
+        <f>E19*D41*B$37</f>
+        <v>2.5302576645721783E-4</v>
+      </c>
+      <c r="G41" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I41" s="1">
+        <v>0.33364751877527898</v>
+      </c>
+      <c r="J41" s="1">
+        <f>I41/G41</f>
+        <v>0.20852969923454936</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+      <c r="H42" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I42" s="1">
+        <v>0.167883773198164</v>
+      </c>
+      <c r="J42" s="1">
+        <f>I42/G41</f>
+        <v>0.10492735824885249</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="32">
+        <v>1</v>
+      </c>
+      <c r="C43" s="5">
+        <f>$C$30</f>
+        <v>1.5</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I43" s="1">
+        <v>2.69894150887699E-4</v>
+      </c>
+      <c r="J43" s="1">
+        <f>I43/G41</f>
+        <v>1.6868384430481187E-4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44" s="9"/>
+      <c r="B44" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="1">
-        <f>C40/D21</f>
+      <c r="C44" s="6"/>
+      <c r="D44" s="1">
+        <f>C43/D21</f>
         <v>1.5</v>
       </c>
-      <c r="E41" s="1">
-        <f>E22*D41*B$40</f>
+      <c r="E44" s="1">
+        <f>E22*D44*B$43</f>
         <v>1.2750000000000001E-4</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B42" s="6" t="s">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B45" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="1">
-        <f>C40/D22</f>
+      <c r="C45" s="6"/>
+      <c r="D45" s="1">
+        <f>C43/D22</f>
         <v>24</v>
       </c>
-      <c r="E42" s="1">
-        <f>E23*D42*B$40</f>
+      <c r="E45" s="1">
+        <f>E23*D45*B$43</f>
         <v>3.0600000000000002E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A43" s="11"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="35" t="s">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="11"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="B44" s="35"/>
-      <c r="C44" s="35"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
-      <c r="H44" s="1" t="s">
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="H47" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="I44" s="1">
+      <c r="I47" s="1">
         <v>0.20852969923454936</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="23"/>
-      <c r="B45" s="24" t="s">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
+      <c r="B48" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="25"/>
-      <c r="I45" s="1">
+      <c r="C48" s="24"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
+      <c r="F48" s="24"/>
+      <c r="G48" s="25"/>
+      <c r="I48" s="1">
         <v>0.10492735824885249</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="26"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="28"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="26"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="28"/>
-      <c r="I47" s="1">
-        <v>1.6868384430481187E-4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" s="26"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="28"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="26"/>
       <c r="B49" s="27"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27" t="str">
-        <f xml:space="preserve"> "MaxEC = " &amp; $C$31</f>
-        <v>MaxEC = 1.5</v>
-      </c>
+      <c r="C49" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D49" s="27"/>
       <c r="E49" s="27"/>
       <c r="F49" s="27"/>
       <c r="G49" s="28"/>
-      <c r="I49" s="1" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="26"/>
       <c r="B50" s="27"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27" t="s">
-        <v>38</v>
-      </c>
+      <c r="C50" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D50" s="27"/>
       <c r="E50" s="27"/>
       <c r="F50" s="27"/>
       <c r="G50" s="28"/>
-      <c r="I50" s="1" t="s">
-        <v>55</v>
+      <c r="I50" s="1">
+        <v>1.6868384430481187E-4</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="26"/>
       <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27" t="s">
+      <c r="C51" s="27" t="s">
         <v>37</v>
       </c>
+      <c r="D51" s="27"/>
       <c r="E51" s="27"/>
       <c r="F51" s="27"/>
       <c r="G51" s="28"/>
-      <c r="I51" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="J51" s="1" t="s">
-        <v>53</v>
-      </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="26"/>
       <c r="B52" s="27"/>
       <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27" t="str">
-        <f xml:space="preserve"> B32 &amp; " = " &amp; E31</f>
-        <v>MonoPropellant = 0.0015</v>
-      </c>
+      <c r="D52" s="27" t="str">
+        <f xml:space="preserve"> "MaxEC = " &amp; $C$34</f>
+        <v>MaxEC = 1.5</v>
+      </c>
+      <c r="E52" s="27"/>
       <c r="F52" s="27"/>
       <c r="G52" s="28"/>
+      <c r="I52" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A53" s="26"/>
       <c r="B53" s="27"/>
       <c r="C53" s="27"/>
       <c r="D53" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E53" s="27"/>
       <c r="F53" s="27"/>
       <c r="G53" s="28"/>
+      <c r="I53" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A54" s="26"/>
       <c r="B54" s="27"/>
-      <c r="C54" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D54" s="27"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="27" t="s">
+        <v>37</v>
+      </c>
       <c r="E54" s="27"/>
       <c r="F54" s="27"/>
       <c r="G54" s="28"/>
+      <c r="I54" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A55" s="26"/>
       <c r="B55" s="27"/>
-      <c r="C55" s="27" t="s">
-        <v>36</v>
-      </c>
+      <c r="C55" s="27"/>
       <c r="D55" s="27"/>
-      <c r="E55" s="27"/>
+      <c r="E55" s="27" t="str">
+        <f xml:space="preserve"> B35 &amp; " = " &amp; E34</f>
+        <v>MonoPropellant = 0.0015</v>
+      </c>
       <c r="F55" s="27"/>
       <c r="G55" s="28"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A56" s="26"/>
       <c r="B56" s="27"/>
-      <c r="C56" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="E56" s="27"/>
       <c r="F56" s="27"/>
       <c r="G56" s="28"/>
@@ -5379,11 +5457,10 @@
     <row r="57" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A57" s="26"/>
       <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27" t="str">
-        <f xml:space="preserve"> "MaxEC = " &amp; $C$27</f>
-        <v>MaxEC = 1.5</v>
-      </c>
+      <c r="C57" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" s="27"/>
       <c r="E57" s="27"/>
       <c r="F57" s="27"/>
       <c r="G57" s="28"/>
@@ -5391,10 +5468,10 @@
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A58" s="26"/>
       <c r="B58" s="27"/>
-      <c r="C58" s="27"/>
-      <c r="D58" s="27" t="s">
-        <v>38</v>
-      </c>
+      <c r="C58" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D58" s="27"/>
       <c r="E58" s="27"/>
       <c r="F58" s="27"/>
       <c r="G58" s="28"/>
@@ -5402,10 +5479,10 @@
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A59" s="26"/>
       <c r="B59" s="27"/>
-      <c r="C59" s="27"/>
-      <c r="D59" s="27" t="s">
+      <c r="C59" s="27" t="s">
         <v>37</v>
       </c>
+      <c r="D59" s="27"/>
       <c r="E59" s="27"/>
       <c r="F59" s="27"/>
       <c r="G59" s="28"/>
@@ -5414,11 +5491,11 @@
       <c r="A60" s="26"/>
       <c r="B60" s="27"/>
       <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
-      <c r="E60" s="27" t="str">
-        <f xml:space="preserve"> B28 &amp; " = " &amp; E28</f>
-        <v>LiquidFuel = 0.0016875</v>
-      </c>
+      <c r="D60" s="27" t="str">
+        <f xml:space="preserve"> "MaxEC = " &amp; $C$30</f>
+        <v>MaxEC = 1.5</v>
+      </c>
+      <c r="E60" s="27"/>
       <c r="F60" s="27"/>
       <c r="G60" s="28"/>
     </row>
@@ -5426,11 +5503,10 @@
       <c r="A61" s="26"/>
       <c r="B61" s="27"/>
       <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
-      <c r="E61" s="27" t="str">
-        <f xml:space="preserve"> B29 &amp; " = " &amp; E29</f>
-        <v>Oxidizer = 0.00458333333333333</v>
-      </c>
+      <c r="D61" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E61" s="27"/>
       <c r="F61" s="27"/>
       <c r="G61" s="28"/>
     </row>
@@ -5439,7 +5515,7 @@
       <c r="B62" s="27"/>
       <c r="C62" s="27"/>
       <c r="D62" s="27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E62" s="27"/>
       <c r="F62" s="27"/>
@@ -5448,32 +5524,34 @@
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A63" s="26"/>
       <c r="B63" s="27"/>
-      <c r="C63" s="27" t="s">
-        <v>39</v>
-      </c>
+      <c r="C63" s="27"/>
       <c r="D63" s="27"/>
-      <c r="E63" s="27"/>
+      <c r="E63" s="27" t="str">
+        <f xml:space="preserve"> B31 &amp; " = " &amp; E31</f>
+        <v>LiquidFuel = 0.0016875</v>
+      </c>
       <c r="F63" s="27"/>
       <c r="G63" s="28"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A64" s="26"/>
       <c r="B64" s="27"/>
-      <c r="C64" s="27" t="s">
-        <v>42</v>
-      </c>
+      <c r="C64" s="27"/>
       <c r="D64" s="27"/>
-      <c r="E64" s="27"/>
+      <c r="E64" s="27" t="str">
+        <f xml:space="preserve"> B32 &amp; " = " &amp; E32</f>
+        <v>Oxidizer = 0.00458333333333333</v>
+      </c>
       <c r="F64" s="27"/>
       <c r="G64" s="28"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="26"/>
       <c r="B65" s="27"/>
-      <c r="C65" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D65" s="27"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="E65" s="27"/>
       <c r="F65" s="27"/>
       <c r="G65" s="28"/>
@@ -5481,11 +5559,10 @@
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="26"/>
       <c r="B66" s="27"/>
-      <c r="C66" s="27"/>
-      <c r="D66" s="27" t="str">
-        <f xml:space="preserve"> "MaxEC = " &amp; $C$34</f>
-        <v>MaxEC = 1.5</v>
-      </c>
+      <c r="C66" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D66" s="27"/>
       <c r="E66" s="27"/>
       <c r="F66" s="27"/>
       <c r="G66" s="28"/>
@@ -5493,10 +5570,10 @@
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="26"/>
       <c r="B67" s="27"/>
-      <c r="C67" s="27"/>
-      <c r="D67" s="27" t="s">
-        <v>38</v>
-      </c>
+      <c r="C67" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="27"/>
       <c r="E67" s="27"/>
       <c r="F67" s="27"/>
       <c r="G67" s="28"/>
@@ -5504,10 +5581,10 @@
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="26"/>
       <c r="B68" s="27"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="27" t="s">
+      <c r="C68" s="27" t="s">
         <v>37</v>
       </c>
+      <c r="D68" s="27"/>
       <c r="E68" s="27"/>
       <c r="F68" s="27"/>
       <c r="G68" s="28"/>
@@ -5516,11 +5593,11 @@
       <c r="A69" s="26"/>
       <c r="B69" s="27"/>
       <c r="C69" s="27"/>
-      <c r="D69" s="27"/>
-      <c r="E69" s="27" t="str">
-        <f xml:space="preserve"> B35 &amp; " = " &amp; E35</f>
-        <v>Hydrogen = 0.312794548851824</v>
-      </c>
+      <c r="D69" s="27" t="str">
+        <f xml:space="preserve"> "MaxEC = " &amp; $C$37</f>
+        <v>MaxEC = 1.5</v>
+      </c>
+      <c r="E69" s="27"/>
       <c r="F69" s="27"/>
       <c r="G69" s="28"/>
     </row>
@@ -5528,11 +5605,10 @@
       <c r="A70" s="26"/>
       <c r="B70" s="27"/>
       <c r="C70" s="27"/>
-      <c r="D70" s="27"/>
-      <c r="E70" s="27" t="str">
-        <f xml:space="preserve"> B36 &amp; " = " &amp; E36</f>
-        <v>Oxygen = 0.236586594765079</v>
-      </c>
+      <c r="D70" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E70" s="27"/>
       <c r="F70" s="27"/>
       <c r="G70" s="28"/>
     </row>
@@ -5541,7 +5617,7 @@
       <c r="B71" s="27"/>
       <c r="C71" s="27"/>
       <c r="D71" s="27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E71" s="27"/>
       <c r="F71" s="27"/>
@@ -5551,10 +5627,11 @@
       <c r="A72" s="26"/>
       <c r="B72" s="27"/>
       <c r="C72" s="27"/>
-      <c r="D72" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="E72" s="27"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="27" t="str">
+        <f xml:space="preserve"> B38 &amp; " = " &amp; E38</f>
+        <v>Hydrogen = 0.312794548851824</v>
+      </c>
       <c r="F72" s="27"/>
       <c r="G72" s="28"/>
     </row>
@@ -5562,10 +5639,11 @@
       <c r="A73" s="26"/>
       <c r="B73" s="27"/>
       <c r="C73" s="27"/>
-      <c r="D73" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="E73" s="27"/>
+      <c r="D73" s="27"/>
+      <c r="E73" s="27" t="str">
+        <f xml:space="preserve"> B39 &amp; " = " &amp; E39</f>
+        <v>Oxygen = 0.236586594765079</v>
+      </c>
       <c r="F73" s="27"/>
       <c r="G73" s="28"/>
     </row>
@@ -5573,11 +5651,10 @@
       <c r="A74" s="26"/>
       <c r="B74" s="27"/>
       <c r="C74" s="27"/>
-      <c r="D74" s="27"/>
-      <c r="E74" s="27" t="str">
-        <f xml:space="preserve"> B38 &amp; " = " &amp; E38</f>
-        <v>Water = 0.000253025766457218</v>
-      </c>
+      <c r="D74" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="E74" s="27"/>
       <c r="F74" s="27"/>
       <c r="G74" s="28"/>
     </row>
@@ -5586,7 +5663,7 @@
       <c r="B75" s="27"/>
       <c r="C75" s="27"/>
       <c r="D75" s="27" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E75" s="27"/>
       <c r="F75" s="27"/>
@@ -5595,10 +5672,10 @@
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="26"/>
       <c r="B76" s="27"/>
-      <c r="C76" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D76" s="27"/>
+      <c r="C76" s="27"/>
+      <c r="D76" s="27" t="s">
+        <v>37</v>
+      </c>
       <c r="E76" s="27"/>
       <c r="F76" s="27"/>
       <c r="G76" s="28"/>
@@ -5606,21 +5683,22 @@
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="26"/>
       <c r="B77" s="27"/>
-      <c r="C77" s="27" t="s">
-        <v>36</v>
-      </c>
+      <c r="C77" s="27"/>
       <c r="D77" s="27"/>
-      <c r="E77" s="27"/>
+      <c r="E77" s="27" t="str">
+        <f xml:space="preserve"> B41 &amp; " = " &amp; E41</f>
+        <v>Water = 0.000253025766457218</v>
+      </c>
       <c r="F77" s="27"/>
       <c r="G77" s="28"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="26"/>
       <c r="B78" s="27"/>
-      <c r="C78" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="D78" s="27"/>
+      <c r="C78" s="27"/>
+      <c r="D78" s="27" t="s">
+        <v>39</v>
+      </c>
       <c r="E78" s="27"/>
       <c r="F78" s="27"/>
       <c r="G78" s="28"/>
@@ -5628,11 +5706,10 @@
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="26"/>
       <c r="B79" s="27"/>
-      <c r="C79" s="27"/>
-      <c r="D79" s="27" t="str">
-        <f xml:space="preserve"> "MaxEC = " &amp; $C$40</f>
-        <v>MaxEC = 1.5</v>
-      </c>
+      <c r="C79" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D79" s="27"/>
       <c r="E79" s="27"/>
       <c r="F79" s="27"/>
       <c r="G79" s="28"/>
@@ -5640,10 +5717,10 @@
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="26"/>
       <c r="B80" s="27"/>
-      <c r="C80" s="27"/>
-      <c r="D80" s="27" t="s">
-        <v>38</v>
-      </c>
+      <c r="C80" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D80" s="27"/>
       <c r="E80" s="27"/>
       <c r="F80" s="27"/>
       <c r="G80" s="28"/>
@@ -5651,10 +5728,10 @@
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="26"/>
       <c r="B81" s="27"/>
-      <c r="C81" s="27"/>
-      <c r="D81" s="27" t="s">
+      <c r="C81" s="27" t="s">
         <v>37</v>
       </c>
+      <c r="D81" s="27"/>
       <c r="E81" s="27"/>
       <c r="F81" s="27"/>
       <c r="G81" s="28"/>
@@ -5663,11 +5740,11 @@
       <c r="A82" s="26"/>
       <c r="B82" s="27"/>
       <c r="C82" s="27"/>
-      <c r="D82" s="27"/>
-      <c r="E82" s="27" t="str">
-        <f xml:space="preserve"> B41 &amp; " = " &amp; E41</f>
-        <v>LiquidFuel = 0.0001275</v>
-      </c>
+      <c r="D82" s="27" t="str">
+        <f xml:space="preserve"> "MaxEC = " &amp; $C$43</f>
+        <v>MaxEC = 1.5</v>
+      </c>
+      <c r="E82" s="27"/>
       <c r="F82" s="27"/>
       <c r="G82" s="28"/>
     </row>
@@ -5675,11 +5752,10 @@
       <c r="A83" s="26"/>
       <c r="B83" s="27"/>
       <c r="C83" s="27"/>
-      <c r="D83" s="27"/>
-      <c r="E83" s="27" t="str">
-        <f xml:space="preserve"> B42 &amp; " = " &amp; E42</f>
-        <v>IntakeAir = 0.0306</v>
-      </c>
+      <c r="D83" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="E83" s="27"/>
       <c r="F83" s="27"/>
       <c r="G83" s="28"/>
     </row>
@@ -5688,7 +5764,7 @@
       <c r="B84" s="27"/>
       <c r="C84" s="27"/>
       <c r="D84" s="27" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E84" s="27"/>
       <c r="F84" s="27"/>
@@ -5697,31 +5773,66 @@
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="26"/>
       <c r="B85" s="27"/>
-      <c r="C85" s="27" t="s">
-        <v>39</v>
-      </c>
+      <c r="C85" s="27"/>
       <c r="D85" s="27"/>
-      <c r="E85" s="27"/>
+      <c r="E85" s="27" t="str">
+        <f xml:space="preserve"> B44 &amp; " = " &amp; E44</f>
+        <v>LiquidFuel = 0.0001275</v>
+      </c>
       <c r="F85" s="27"/>
       <c r="G85" s="28"/>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A86" s="29"/>
-      <c r="B86" s="30" t="s">
+      <c r="A86" s="26"/>
+      <c r="B86" s="27"/>
+      <c r="C86" s="27"/>
+      <c r="D86" s="27"/>
+      <c r="E86" s="27" t="str">
+        <f xml:space="preserve"> B45 &amp; " = " &amp; E45</f>
+        <v>IntakeAir = 0.0306</v>
+      </c>
+      <c r="F86" s="27"/>
+      <c r="G86" s="28"/>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A87" s="26"/>
+      <c r="B87" s="27"/>
+      <c r="C87" s="27"/>
+      <c r="D87" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="C86" s="30"/>
-      <c r="D86" s="30"/>
-      <c r="E86" s="30"/>
-      <c r="F86" s="30"/>
-      <c r="G86" s="31"/>
+      <c r="E87" s="27"/>
+      <c r="F87" s="27"/>
+      <c r="G87" s="28"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="26"/>
+      <c r="B88" s="27"/>
+      <c r="C88" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D88" s="27"/>
+      <c r="E88" s="27"/>
+      <c r="F88" s="27"/>
+      <c r="G88" s="28"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="29"/>
+      <c r="B89" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C89" s="30"/>
+      <c r="D89" s="30"/>
+      <c r="E89" s="30"/>
+      <c r="F89" s="30"/>
+      <c r="G89" s="31"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A44:E44"/>
+    <mergeCell ref="A47:E47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>